<commit_message>
added data gthat fit poisson distribution
</commit_message>
<xml_diff>
--- a/data/data_supermarket.xlsx
+++ b/data/data_supermarket.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F460078-17EC-4B1B-9115-D53D7519888D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{74195566-0079-4324-9CCE-E5064B2D4687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>lower range</t>
   </si>
@@ -44,12 +44,66 @@
   <si>
     <t>Totale range</t>
   </si>
+  <si>
+    <t>VALIDAZIONE DEI DATI</t>
+  </si>
+  <si>
+    <t>classe</t>
+  </si>
+  <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>Totale</t>
+  </si>
+  <si>
+    <t>ris</t>
+  </si>
+  <si>
+    <t>p(i)</t>
+  </si>
+  <si>
+    <t>Fi</t>
+  </si>
+  <si>
+    <t>Fi raggruppato</t>
+  </si>
+  <si>
+    <t>fi raggruppato</t>
+  </si>
+  <si>
+    <t>Gi</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>DF = 13-1-1</t>
+  </si>
+  <si>
+    <t>SOMME</t>
+  </si>
+  <si>
+    <t>Tra p10 e P90</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>varianza</t>
+  </si>
+  <si>
+    <t>dev std</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,8 +119,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +158,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -104,13 +177,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,7 +240,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>observed frequency</a:t>
+              <a:t>OBSERVED FREQUENCY</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -217,20 +294,128 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$4:$C$19</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="16"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>16:15</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>16:30</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16:45</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>17:00</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>17:15</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>17:30</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>17:45</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>18:00</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>18:15</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>18:30</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>18:45</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>19:00</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19:15</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>19:30</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>19:45</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>20:00</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>16:00</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>16:15</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>16:30</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>16:45</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>17:00</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>17:15</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>17:30</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>17:45</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>18:00</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>18:15</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>18:30</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>18:45</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>19:00</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>19:15</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>19:30</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>19:45</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$18</c:f>
+              <c:f>Sheet1!$D$4:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7</c:v>
@@ -239,41 +424,44 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-F2C4-424E-85C0-B59E17253120}"/>
+              <c16:uniqueId val="{00000001-7B4C-495D-A8E4-28AE24221FF4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -287,16 +475,17 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1131918311"/>
-        <c:axId val="1131913991"/>
+        <c:axId val="1859426663"/>
+        <c:axId val="1859442983"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1131918311"/>
+        <c:axId val="1859426663"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -333,7 +522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1131913991"/>
+        <c:crossAx val="1859442983"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -341,7 +530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1131913991"/>
+        <c:axId val="1859442983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,7 +581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1131918311"/>
+        <c:crossAx val="1859426663"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -406,6 +595,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.44639064453118754"/>
+          <c:y val="0.93544823308464997"/>
+          <c:w val="7.0677907039939133E-2"/>
+          <c:h val="4.9234480263271256E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1019,26 +1218,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{565F8ADD-E32E-E4EF-E04F-B381E8FFE30D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41DEA6F9-D674-CDE2-CB1C-1F891ECB1515}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3A142266-ACA3-CCE3-74DE-160F31D31D6F}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{565F8ADD-E32E-E4EF-E04F-B381E8FFE30D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1356,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:D21"/>
+  <dimension ref="A3:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1389,7 +1588,7 @@
         <v>0.67708333333333337</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:4">
@@ -1400,7 +1599,7 @@
         <v>0.6875</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:4">
@@ -1411,7 +1610,7 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="D6">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -1444,7 +1643,7 @@
         <v>0.72916666666666696</v>
       </c>
       <c r="D9">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -1455,7 +1654,7 @@
         <v>0.73958333333333304</v>
       </c>
       <c r="D10">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -1466,7 +1665,7 @@
         <v>0.75</v>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -1477,7 +1676,7 @@
         <v>0.76041666666666596</v>
       </c>
       <c r="D12">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -1499,7 +1698,7 @@
         <v>0.781249999999999</v>
       </c>
       <c r="D14">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -1510,7 +1709,7 @@
         <v>0.79166666666666596</v>
       </c>
       <c r="D15">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -1521,10 +1720,10 @@
         <v>0.80208333333333304</v>
       </c>
       <c r="D16">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="B17" s="1">
         <v>0.80208333333333504</v>
       </c>
@@ -1532,10 +1731,10 @@
         <v>0.812499999999999</v>
       </c>
       <c r="D17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="B18" s="1">
         <v>0.812500000000001</v>
       </c>
@@ -1543,10 +1742,10 @@
         <v>0.82291666666666596</v>
       </c>
       <c r="D18">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="B19" s="1">
         <v>0.82291666666666796</v>
       </c>
@@ -1554,15 +1753,15 @@
         <v>0.83333333333333204</v>
       </c>
       <c r="D19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="D20" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:10">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1572,7 +1771,670 @@
       </c>
       <c r="D21" s="5">
         <f>SUM(D4:D19)</f>
-        <v>155</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="B27" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" s="8"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="B28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <f>C29*B29</f>
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <f>((B29-$C$48)^2)*C29</f>
+        <v>55.635250516044287</v>
+      </c>
+      <c r="F29">
+        <f>(EXP(-$C$48)*$C$48^B29)/FACT(B29)</f>
+        <v>5.7628737336649005E-4</v>
+      </c>
+      <c r="G29">
+        <f>$C$46*F29</f>
+        <v>8.4137956511507545E-2</v>
+      </c>
+      <c r="H29">
+        <f>SUM(G29:G30)</f>
+        <v>0.71171490610761523</v>
+      </c>
+      <c r="I29">
+        <f>SUM(C29:C30)</f>
+        <v>3</v>
+      </c>
+      <c r="J29">
+        <f>((I29-H29)^2)/H29</f>
+        <v>7.3572277691459922</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:D44" si="0">C30*B30</f>
+        <v>2</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ref="E30:E44" si="1">((B30-$C$48)^2)*C30</f>
+        <v>83.43488459373242</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ref="F30:F44" si="2">(EXP(-$C$48)*$C$48^B30)/FACT(B30)</f>
+        <v>4.2984722575075867E-3</v>
+      </c>
+      <c r="G30">
+        <f t="shared" ref="G30:G44" si="3">$C$46*F30</f>
+        <v>0.62757694959610766</v>
+      </c>
+      <c r="H30">
+        <f>G31</f>
+        <v>2.3405181442128811</v>
+      </c>
+      <c r="I30">
+        <f>C31</f>
+        <v>5</v>
+      </c>
+      <c r="J30">
+        <f t="shared" ref="J30:J41" si="4">((I30-H30)^2)/H30</f>
+        <v>3.02191365563607</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>148.99817038844063</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>1.6030946193238912E-2</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="3"/>
+        <v>2.3405181442128811</v>
+      </c>
+      <c r="H31">
+        <f t="shared" ref="H31:H41" si="5">G32</f>
+        <v>5.8192334681457245</v>
+      </c>
+      <c r="I31">
+        <f t="shared" ref="I31:I40" si="6">C32</f>
+        <v>7</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="4"/>
+        <v>0.23958646965773536</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>139.17278100957029</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>3.985776348045017E-2</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="3"/>
+        <v>5.8192334681457245</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="5"/>
+        <v>10.851276107552557</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="4"/>
+        <v>6.6782100474381781E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>119.64017639331959</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>7.432380895583944E-2</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="3"/>
+        <v>10.851276107552557</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="5"/>
+        <v>16.187725590581831</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="4"/>
+        <v>8.7145786517638574E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="B34">
+        <v>5</v>
+      </c>
+      <c r="C34">
+        <v>15</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>90.693141302308149</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>0.11087483281220432</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="3"/>
+        <v>16.187725590581831</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="5"/>
+        <v>20.123782155415089</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="4"/>
+        <v>1.8635019797652324</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="B35">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>29.797616813661108</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>0.13783412435215814</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="3"/>
+        <v>20.123782155415089</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="5"/>
+        <v>21.443051631357175</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="4"/>
+        <v>9.1542356667743685E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="B36">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>21</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>147</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>4.4224526177519294</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>0.14687021665313132</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="3"/>
+        <v>21.443051631357175</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="5"/>
+        <v>19.992708241907501</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="6"/>
+        <v>17</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="4"/>
+        <v>0.44797845858658736</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="B37">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>17</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>136</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>4.9773409645336786</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>0.13693635782128424</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="3"/>
+        <v>19.992708241907501</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="5"/>
+        <v>16.569299296375394</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="4"/>
+        <v>0.14863032150931299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="B38">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>15</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>35.624648151623177</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>0.11348835134503694</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="3"/>
+        <v>16.569299296375394</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="5"/>
+        <v>12.358881461474521</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="4"/>
+        <v>0.56441249608932842</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>96.857524863951937</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>8.4649873023798089E-2</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="3"/>
+        <v>12.358881461474521</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="5"/>
+        <v>8.3803374293560111</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="4"/>
+        <v>0.31303117146044113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="B40">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>110</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>125.3936010508538</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="2"/>
+        <v>5.7399571433945286E-2</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="3"/>
+        <v>8.3803374293560111</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="5"/>
+        <v>5.209011107630535</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="4"/>
+        <v>0.6157869788167698</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="B41">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>144.35086320135107</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="2"/>
+        <v>3.5678158271442023E-2</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="3"/>
+        <v>5.209011107630535</v>
+      </c>
+      <c r="H41">
+        <f>SUM(G42:G44)</f>
+        <v>5.3728690800432704</v>
+      </c>
+      <c r="I41">
+        <f>SUM(C42:C44)</f>
+        <v>7</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="4"/>
+        <v>0.49276373409379842</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="B42">
+        <v>13</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>122.81497466691685</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="2"/>
+        <v>2.0470766257955932E-2</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="3"/>
+        <v>2.9887318736615662</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="B43">
+        <v>14</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>85.571870895102265</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="2"/>
+        <v>1.0906391611993155E-2</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="3"/>
+        <v>1.5923331753510006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="B44">
+        <v>15</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>56.868127228373048</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="2"/>
+        <v>5.4233152810322137E-3</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="3"/>
+        <v>0.79180403103070318</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="J45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9">
+        <f>SUM(C29:C44)</f>
+        <v>146</v>
+      </c>
+      <c r="D46" s="9">
+        <f t="shared" ref="D46:J46" si="7">SUM(D29:D44)</f>
+        <v>1089</v>
+      </c>
+      <c r="E46" s="9">
+        <f t="shared" si="7"/>
+        <v>1344.253424657534</v>
+      </c>
+      <c r="F46" s="9">
+        <f t="shared" si="7"/>
+        <v>0.99561923712438427</v>
+      </c>
+      <c r="G46" s="9">
+        <f t="shared" si="7"/>
+        <v>145.36040862016011</v>
+      </c>
+      <c r="H46" s="9">
+        <f t="shared" si="7"/>
+        <v>145.36040862016011</v>
+      </c>
+      <c r="I46" s="9">
+        <f t="shared" si="7"/>
+        <v>146</v>
+      </c>
+      <c r="J46" s="9">
+        <f t="shared" si="7"/>
+        <v>15.227915157420062</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="J47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="B48" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C48" s="6">
+        <f>D46/C46</f>
+        <v>7.4589041095890414</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3">
+      <c r="B49" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="6">
+        <f>E46/(C46-1)</f>
+        <v>9.2707132735002347</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3">
+      <c r="B50" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="6">
+        <f>SQRT(C49)</f>
+        <v>3.0447846021517244</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3">
+      <c r="B51" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="6">
+        <f>C50/C48</f>
+        <v>0.40820803665211364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added validated data with typo fixed and notes
</commit_message>
<xml_diff>
--- a/data/data_supermarket.xlsx
+++ b/data/data_supermarket.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26207"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74195566-0079-4324-9CCE-E5064B2D4687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A186A5E9-AA50-48F5-A3F0-B0483A108646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="25">
   <si>
     <t>lower range</t>
   </si>
@@ -98,6 +99,12 @@
   <si>
     <t>v</t>
   </si>
+  <si>
+    <t>lamda</t>
+  </si>
+  <si>
+    <t>DF = 12-1-1</t>
+  </si>
 </sst>
 </file>
 
@@ -133,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +171,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -177,7 +190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -188,6 +201,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,43 +429,43 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>14</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>17</c:v>
-                </c:pt>
                 <c:pt idx="9">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1</c:v>
@@ -671,7 +685,369 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$9:$F$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BCC4-4228-89A4-AB475FDE5A87}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1002348183"/>
+        <c:axId val="1002351063"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1002348183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1002351063"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1002351063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1002348183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1214,6 +1590,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1238,6 +2117,47 @@
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{565F8ADD-E32E-E4EF-E04F-B381E8FFE30D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4529A858-A01F-3890-FD7C-D42CA87C6AB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1555,10 +2475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:L51"/>
+  <dimension ref="A3:AB52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1610,7 +2530,7 @@
         <v>0.69791666666666696</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:4">
@@ -1632,7 +2552,7 @@
         <v>0.71875</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:4">
@@ -1643,7 +2563,7 @@
         <v>0.72916666666666696</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:4">
@@ -1654,7 +2574,7 @@
         <v>0.73958333333333304</v>
       </c>
       <c r="D10">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:4">
@@ -1665,7 +2585,7 @@
         <v>0.75</v>
       </c>
       <c r="D11">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:4">
@@ -1676,7 +2596,7 @@
         <v>0.76041666666666596</v>
       </c>
       <c r="D12">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:4">
@@ -1687,7 +2607,7 @@
         <v>0.77083333333333304</v>
       </c>
       <c r="D13">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:4">
@@ -1698,7 +2618,7 @@
         <v>0.781249999999999</v>
       </c>
       <c r="D14">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:4">
@@ -1709,7 +2629,7 @@
         <v>0.79166666666666596</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:4">
@@ -1720,10 +2640,10 @@
         <v>0.80208333333333304</v>
       </c>
       <c r="D16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
       <c r="B17" s="1">
         <v>0.80208333333333504</v>
       </c>
@@ -1731,10 +2651,10 @@
         <v>0.812499999999999</v>
       </c>
       <c r="D17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
       <c r="B18" s="1">
         <v>0.812500000000001</v>
       </c>
@@ -1742,10 +2662,10 @@
         <v>0.82291666666666596</v>
       </c>
       <c r="D18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
       <c r="B19" s="1">
         <v>0.82291666666666796</v>
       </c>
@@ -1756,12 +2676,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:26">
       <c r="D20" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:26">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1771,16 +2691,20 @@
       </c>
       <c r="D21" s="5">
         <f>SUM(D4:D19)</f>
-        <v>146</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
       <c r="B27" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:10">
+      <c r="R27" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="S27" s="8"/>
+    </row>
+    <row r="28" spans="1:26">
       <c r="B28" s="5" t="s">
         <v>6</v>
       </c>
@@ -1808,8 +2732,35 @@
       <c r="J28" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="1:10">
+      <c r="R28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="S28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="T28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="U28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="V28" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="W28" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="X28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z28" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
       <c r="B29">
         <v>0</v>
       </c>
@@ -1844,8 +2795,42 @@
         <f>((I29-H29)^2)/H29</f>
         <v>7.3572277691459922</v>
       </c>
-    </row>
-    <row r="30" spans="1:10">
+      <c r="R29">
+        <v>0</v>
+      </c>
+      <c r="S29">
+        <v>1</v>
+      </c>
+      <c r="T29">
+        <f>S29*R29</f>
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <f>((R29-$C$48)^2)*S29</f>
+        <v>55.635250516044287</v>
+      </c>
+      <c r="V29">
+        <f>(EXP(-$S$52)*$S$52^R29)/FACT(R29)</f>
+        <v>2.3292158839187684E-4</v>
+      </c>
+      <c r="W29">
+        <f>$C$46*V29</f>
+        <v>3.4006551905214018E-2</v>
+      </c>
+      <c r="X29">
+        <f>SUM(W29:W30)</f>
+        <v>0.31846485285141213</v>
+      </c>
+      <c r="Y29">
+        <f>SUM(S29:S30)</f>
+        <v>3</v>
+      </c>
+      <c r="Z29">
+        <f>((Y29-X29)^2)/X29</f>
+        <v>22.579040296004564</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
       <c r="B30">
         <v>1</v>
       </c>
@@ -1880,8 +2865,42 @@
         <f t="shared" ref="J30:J41" si="4">((I30-H30)^2)/H30</f>
         <v>3.02191365563607</v>
       </c>
-    </row>
-    <row r="31" spans="1:10">
+      <c r="R30">
+        <v>1</v>
+      </c>
+      <c r="S30">
+        <v>2</v>
+      </c>
+      <c r="T30">
+        <f t="shared" ref="T30:T44" si="5">S30*R30</f>
+        <v>2</v>
+      </c>
+      <c r="U30">
+        <f t="shared" ref="U30:U44" si="6">((R30-$C$48)^2)*S30</f>
+        <v>83.43488459373242</v>
+      </c>
+      <c r="V30">
+        <f t="shared" ref="V30:V44" si="7">(EXP(-$S$52)*$S$52^R30)/FACT(R30)</f>
+        <v>1.948344527028754E-3</v>
+      </c>
+      <c r="W30">
+        <f t="shared" ref="W30:W44" si="8">$C$46*V30</f>
+        <v>0.28445830094619812</v>
+      </c>
+      <c r="X30">
+        <f>W31</f>
+        <v>1.1897196340683891</v>
+      </c>
+      <c r="Y30">
+        <f>S31</f>
+        <v>5</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" ref="Z30:Z41" si="9">((Y30-X30)^2)/X30</f>
+        <v>12.203073775757636</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
       <c r="B31">
         <v>2</v>
       </c>
@@ -1905,19 +2924,53 @@
         <v>2.3405181442128811</v>
       </c>
       <c r="H31">
-        <f t="shared" ref="H31:H41" si="5">G32</f>
+        <f t="shared" ref="H31:H41" si="10">G32</f>
         <v>5.8192334681457245</v>
       </c>
       <c r="I31">
-        <f t="shared" ref="I31:I40" si="6">C32</f>
+        <f t="shared" ref="I31:I40" si="11">C32</f>
         <v>7</v>
       </c>
       <c r="J31">
         <f t="shared" si="4"/>
         <v>0.23958646965773536</v>
       </c>
-    </row>
-    <row r="32" spans="1:10">
+      <c r="R31">
+        <v>2</v>
+      </c>
+      <c r="S31">
+        <v>5</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="6"/>
+        <v>148.99817038844063</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="7"/>
+        <v>8.148764616906775E-3</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="8"/>
+        <v>1.1897196340683891</v>
+      </c>
+      <c r="X31">
+        <f t="shared" ref="X31:X41" si="12">W32</f>
+        <v>3.3172590451855224</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" ref="Y31:Y40" si="13">S32</f>
+        <v>7</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="9"/>
+        <v>4.0884901527216559</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26">
       <c r="B32">
         <v>3</v>
       </c>
@@ -1941,19 +2994,53 @@
         <v>5.8192334681457245</v>
       </c>
       <c r="H32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>10.851276107552557</v>
       </c>
       <c r="I32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="J32">
         <f t="shared" si="4"/>
         <v>6.6782100474381781E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:12">
+      <c r="R32">
+        <v>3</v>
+      </c>
+      <c r="S32">
+        <v>7</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="6"/>
+        <v>139.17278100957029</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="7"/>
+        <v>2.27209523642844E-2</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="8"/>
+        <v>3.3172590451855224</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="12"/>
+        <v>6.9370593233182323</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="9"/>
+        <v>1.3523894133839156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28">
       <c r="B33">
         <v>4</v>
       </c>
@@ -1977,19 +3064,53 @@
         <v>10.851276107552557</v>
       </c>
       <c r="H33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>16.187725590581831</v>
       </c>
       <c r="I33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
       <c r="J33">
         <f t="shared" si="4"/>
         <v>8.7145786517638574E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:12">
+      <c r="R33">
+        <v>4</v>
+      </c>
+      <c r="S33">
+        <v>10</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="6"/>
+        <v>119.64017639331959</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="7"/>
+        <v>4.7514104954234471E-2</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="8"/>
+        <v>6.9370593233182323</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="12"/>
+        <v>11.605434824290626</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="9"/>
+        <v>0.99290314465603435</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28">
       <c r="B34">
         <v>5</v>
       </c>
@@ -2013,19 +3134,53 @@
         <v>16.187725590581831</v>
       </c>
       <c r="H34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>20.123782155415089</v>
       </c>
       <c r="I34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>14</v>
       </c>
       <c r="J34">
         <f t="shared" si="4"/>
         <v>1.8635019797652324</v>
       </c>
-    </row>
-    <row r="35" spans="1:12">
+      <c r="R34">
+        <v>5</v>
+      </c>
+      <c r="S34">
+        <v>15</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="6"/>
+        <v>90.693141302308149</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="7"/>
+        <v>7.9489279618428943E-2</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="8"/>
+        <v>11.605434824290626</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="12"/>
+        <v>16.17954034789684</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="13"/>
+        <v>14</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="9"/>
+        <v>0.29360513500173541</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28">
       <c r="B35">
         <v>6</v>
       </c>
@@ -2049,19 +3204,53 @@
         <v>20.123782155415089</v>
       </c>
       <c r="H35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>21.443051631357175</v>
       </c>
       <c r="I35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>21</v>
       </c>
       <c r="J35">
         <f t="shared" si="4"/>
         <v>9.1542356667743685E-3</v>
       </c>
-    </row>
-    <row r="36" spans="1:12">
+      <c r="R35">
+        <v>6</v>
+      </c>
+      <c r="S35">
+        <v>14</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="5"/>
+        <v>84</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="6"/>
+        <v>29.797616813661108</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="7"/>
+        <v>0.11081876950614274</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="8"/>
+        <v>16.17954034789684</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="12"/>
+        <v>19.334108532469237</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="13"/>
+        <v>21</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" si="9"/>
+        <v>0.1435387815751217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28">
       <c r="B36">
         <v>7</v>
       </c>
@@ -2085,19 +3274,53 @@
         <v>21.443051631357175</v>
       </c>
       <c r="H36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>19.992708241907501</v>
       </c>
       <c r="I36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>17</v>
       </c>
       <c r="J36">
         <f t="shared" si="4"/>
         <v>0.44797845858658736</v>
       </c>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="R36">
+        <v>7</v>
+      </c>
+      <c r="S36">
+        <v>21</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="5"/>
+        <v>147</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="6"/>
+        <v>4.4224526177519294</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="7"/>
+        <v>0.13242540090732355</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="8"/>
+        <v>19.334108532469237</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="12"/>
+        <v>20.215764886958254</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="13"/>
+        <v>17</v>
+      </c>
+      <c r="Z36">
+        <f t="shared" si="9"/>
+        <v>0.51153858713824829</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28">
       <c r="B37">
         <v>8</v>
       </c>
@@ -2121,19 +3344,53 @@
         <v>19.992708241907501</v>
       </c>
       <c r="H37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>16.569299296375394</v>
       </c>
       <c r="I37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
       <c r="J37">
         <f t="shared" si="4"/>
         <v>0.14863032150931299</v>
       </c>
-    </row>
-    <row r="38" spans="1:12">
+      <c r="R37">
+        <v>8</v>
+      </c>
+      <c r="S37">
+        <v>17</v>
+      </c>
+      <c r="T37">
+        <f t="shared" si="5"/>
+        <v>136</v>
+      </c>
+      <c r="U37">
+        <f t="shared" si="6"/>
+        <v>4.9773409645336786</v>
+      </c>
+      <c r="V37">
+        <f t="shared" si="7"/>
+        <v>0.1384641430613579</v>
+      </c>
+      <c r="W37">
+        <f t="shared" si="8"/>
+        <v>20.215764886958254</v>
+      </c>
+      <c r="X37">
+        <f t="shared" si="12"/>
+        <v>18.789000648072367</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" si="9"/>
+        <v>0.76409204406332842</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28">
       <c r="B38">
         <v>9</v>
       </c>
@@ -2157,19 +3414,53 @@
         <v>16.569299296375394</v>
       </c>
       <c r="H38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>12.358881461474521</v>
       </c>
       <c r="I38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>15</v>
       </c>
       <c r="J38">
         <f t="shared" si="4"/>
         <v>0.56441249608932842</v>
       </c>
-    </row>
-    <row r="39" spans="1:12">
+      <c r="R38">
+        <v>9</v>
+      </c>
+      <c r="S38">
+        <v>15</v>
+      </c>
+      <c r="T38">
+        <f t="shared" si="5"/>
+        <v>135</v>
+      </c>
+      <c r="U38">
+        <f t="shared" si="6"/>
+        <v>35.624648151623177</v>
+      </c>
+      <c r="V38">
+        <f t="shared" si="7"/>
+        <v>0.12869178526076963</v>
+      </c>
+      <c r="W38">
+        <f t="shared" si="8"/>
+        <v>18.789000648072367</v>
+      </c>
+      <c r="X38">
+        <f t="shared" si="12"/>
+        <v>15.716639592643359</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" si="9"/>
+        <v>3.2676979243351265E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28">
       <c r="B39">
         <v>10</v>
       </c>
@@ -2193,19 +3484,53 @@
         <v>12.358881461474521</v>
       </c>
       <c r="H39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>8.3803374293560111</v>
       </c>
       <c r="I39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>10</v>
       </c>
       <c r="J39">
         <f t="shared" si="4"/>
         <v>0.31303117146044113</v>
       </c>
-    </row>
-    <row r="40" spans="1:12">
+      <c r="R39">
+        <v>10</v>
+      </c>
+      <c r="S39">
+        <v>15</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="5"/>
+        <v>150</v>
+      </c>
+      <c r="U39">
+        <f t="shared" si="6"/>
+        <v>96.857524863951937</v>
+      </c>
+      <c r="V39">
+        <f t="shared" si="7"/>
+        <v>0.10764821638796822</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="8"/>
+        <v>15.716639592643359</v>
+      </c>
+      <c r="X39">
+        <f t="shared" si="12"/>
+        <v>11.951516678765248</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" si="13"/>
+        <v>10</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" si="9"/>
+        <v>0.31865556898443836</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28">
       <c r="B40">
         <v>11</v>
       </c>
@@ -2229,19 +3554,53 @@
         <v>8.3803374293560111</v>
       </c>
       <c r="H40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>5.209011107630535</v>
       </c>
       <c r="I40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>7</v>
       </c>
       <c r="J40">
         <f t="shared" si="4"/>
         <v>0.6157869788167698</v>
       </c>
-    </row>
-    <row r="41" spans="1:12">
+      <c r="R40">
+        <v>11</v>
+      </c>
+      <c r="S40">
+        <v>10</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="5"/>
+        <v>110</v>
+      </c>
+      <c r="U40">
+        <f t="shared" si="6"/>
+        <v>125.3936010508538</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="7"/>
+        <v>8.1859703279214033E-2</v>
+      </c>
+      <c r="W40">
+        <f t="shared" si="8"/>
+        <v>11.951516678765248</v>
+      </c>
+      <c r="X40">
+        <f t="shared" si="12"/>
+        <v>8.3310125493063563</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" si="9"/>
+        <v>0.21265055068948482</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28">
       <c r="B41">
         <v>12</v>
       </c>
@@ -2276,8 +3635,42 @@
         <f t="shared" si="4"/>
         <v>0.49276373409379842</v>
       </c>
-    </row>
-    <row r="42" spans="1:12">
+      <c r="R41">
+        <v>12</v>
+      </c>
+      <c r="S41">
+        <v>7</v>
+      </c>
+      <c r="T41">
+        <f t="shared" si="5"/>
+        <v>84</v>
+      </c>
+      <c r="U41">
+        <f t="shared" si="6"/>
+        <v>144.35086320135107</v>
+      </c>
+      <c r="V41">
+        <f t="shared" si="7"/>
+        <v>5.7061729789769568E-2</v>
+      </c>
+      <c r="W41">
+        <f t="shared" si="8"/>
+        <v>8.3310125493063563</v>
+      </c>
+      <c r="X41">
+        <f>SUM(W42:W44)</f>
+        <v>10.349516370237094</v>
+      </c>
+      <c r="Y41">
+        <f>SUM(S42:S44)</f>
+        <v>7</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" si="9"/>
+        <v>1.0840371195267029</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28">
       <c r="B42">
         <v>13</v>
       </c>
@@ -2300,8 +3693,30 @@
         <f t="shared" si="3"/>
         <v>2.9887318736615662</v>
       </c>
-    </row>
-    <row r="43" spans="1:12">
+      <c r="R42">
+        <v>13</v>
+      </c>
+      <c r="S42">
+        <v>4</v>
+      </c>
+      <c r="T42">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="U42">
+        <f t="shared" si="6"/>
+        <v>122.81497466691685</v>
+      </c>
+      <c r="V42">
+        <f t="shared" si="7"/>
+        <v>3.6716188715387392E-2</v>
+      </c>
+      <c r="W42">
+        <f t="shared" si="8"/>
+        <v>5.3605635524465596</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
       <c r="B43">
         <v>14</v>
       </c>
@@ -2324,8 +3739,30 @@
         <f t="shared" si="3"/>
         <v>1.5923331753510006</v>
       </c>
-    </row>
-    <row r="44" spans="1:12">
+      <c r="R43">
+        <v>14</v>
+      </c>
+      <c r="S43">
+        <v>2</v>
+      </c>
+      <c r="T43">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="U43">
+        <f t="shared" si="6"/>
+        <v>85.571870895102265</v>
+      </c>
+      <c r="V43">
+        <f t="shared" si="7"/>
+        <v>2.1937421034776115E-2</v>
+      </c>
+      <c r="W43">
+        <f t="shared" si="8"/>
+        <v>3.202863471077313</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28">
       <c r="B44">
         <v>15</v>
       </c>
@@ -2348,8 +3785,30 @@
         <f t="shared" si="3"/>
         <v>0.79180403103070318</v>
       </c>
-    </row>
-    <row r="45" spans="1:12">
+      <c r="R44">
+        <v>15</v>
+      </c>
+      <c r="S44">
+        <v>1</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="U44">
+        <f t="shared" si="6"/>
+        <v>56.868127228373048</v>
+      </c>
+      <c r="V44">
+        <f t="shared" si="7"/>
+        <v>1.2233488676117963E-2</v>
+      </c>
+      <c r="W44">
+        <f t="shared" si="8"/>
+        <v>1.7860893467132226</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28">
       <c r="J45" s="3" t="s">
         <v>15</v>
       </c>
@@ -2357,8 +3816,15 @@
       <c r="L45" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="Z45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AA45" s="3"/>
+      <c r="AB45" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28">
       <c r="A46" s="9" t="s">
         <v>17</v>
       </c>
@@ -2368,40 +3834,79 @@
         <v>146</v>
       </c>
       <c r="D46" s="9">
-        <f t="shared" ref="D46:J46" si="7">SUM(D29:D44)</f>
+        <f t="shared" ref="D46:J46" si="14">SUM(D29:D44)</f>
         <v>1089</v>
       </c>
       <c r="E46" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>1344.253424657534</v>
       </c>
       <c r="F46" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>0.99561923712438427</v>
       </c>
       <c r="G46" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>145.36040862016011</v>
       </c>
       <c r="H46" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>145.36040862016011</v>
       </c>
       <c r="I46" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>146</v>
       </c>
       <c r="J46" s="9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="14"/>
         <v>15.227915157420062</v>
       </c>
-    </row>
-    <row r="47" spans="1:12">
+      <c r="Q46" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R46" s="9"/>
+      <c r="S46" s="9">
+        <f>SUM(S29:S44)</f>
+        <v>146</v>
+      </c>
+      <c r="T46" s="9">
+        <f t="shared" ref="T46:Z46" si="15">SUM(T29:T44)</f>
+        <v>1089</v>
+      </c>
+      <c r="U46" s="9">
+        <f t="shared" si="15"/>
+        <v>1344.253424657534</v>
+      </c>
+      <c r="V46" s="9">
+        <f t="shared" si="15"/>
+        <v>0.98791121428810225</v>
+      </c>
+      <c r="W46" s="9">
+        <f t="shared" si="15"/>
+        <v>144.23503728606295</v>
+      </c>
+      <c r="X46" s="9">
+        <f t="shared" si="15"/>
+        <v>144.23503728606295</v>
+      </c>
+      <c r="Y46" s="9">
+        <f t="shared" si="15"/>
+        <v>146</v>
+      </c>
+      <c r="Z46" s="9">
+        <f t="shared" si="15"/>
+        <v>44.576691548746211</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28">
       <c r="J47" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="1:12">
+      <c r="Z47" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28">
       <c r="B48" s="6" t="s">
         <v>19</v>
       </c>
@@ -2409,8 +3914,15 @@
         <f>D46/C46</f>
         <v>7.4589041095890414</v>
       </c>
-    </row>
-    <row r="49" spans="2:3">
+      <c r="R48" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S48" s="6">
+        <f>T46/S46</f>
+        <v>7.4589041095890414</v>
+      </c>
+    </row>
+    <row r="49" spans="2:19">
       <c r="B49" s="6" t="s">
         <v>20</v>
       </c>
@@ -2418,8 +3930,15 @@
         <f>E46/(C46-1)</f>
         <v>9.2707132735002347</v>
       </c>
-    </row>
-    <row r="50" spans="2:3">
+      <c r="R49" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S49" s="6">
+        <f>U46/(S46-1)</f>
+        <v>9.2707132735002347</v>
+      </c>
+    </row>
+    <row r="50" spans="2:19">
       <c r="B50" s="6" t="s">
         <v>21</v>
       </c>
@@ -2427,14 +3946,713 @@
         <f>SQRT(C49)</f>
         <v>3.0447846021517244</v>
       </c>
-    </row>
-    <row r="51" spans="2:3">
+      <c r="R50" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S50" s="6">
+        <f>SQRT(S49)</f>
+        <v>3.0447846021517244</v>
+      </c>
+    </row>
+    <row r="51" spans="2:19">
       <c r="B51" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C51" s="6">
         <f>C50/C48</f>
         <v>0.40820803665211364</v>
+      </c>
+      <c r="R51" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S51" s="6">
+        <f>S50/S48</f>
+        <v>0.40820803665211364</v>
+      </c>
+    </row>
+    <row r="52" spans="2:19">
+      <c r="R52" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="S52" s="10">
+        <f>(S48+S49)/2</f>
+        <v>8.3648086915446385</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30E074A-9AFA-4A82-A605-A02C2F731617}">
+  <dimension ref="D7:O32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9:F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="7" spans="5:13">
+      <c r="E7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="5:13">
+      <c r="E8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="5:13">
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <f>F9*E9</f>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>((E9-$F$28)^2)*F9</f>
+        <v>50.141709276844409</v>
+      </c>
+      <c r="I9">
+        <f>(EXP(-$F$32)*$F$32^E9)/FACT(E9)</f>
+        <v>4.3450081336133596E-4</v>
+      </c>
+      <c r="J9">
+        <f>$F$26*I9</f>
+        <v>6.4306120377477724E-2</v>
+      </c>
+      <c r="K9">
+        <f>SUM(J9:J11)</f>
+        <v>2.4889860232807921</v>
+      </c>
+      <c r="L9">
+        <f>SUM(F9:F11)</f>
+        <v>7</v>
+      </c>
+      <c r="M9">
+        <f>((L9-K9)^2)/K9</f>
+        <v>8.1757177050489069</v>
+      </c>
+    </row>
+    <row r="10" spans="5:13">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ref="G10:G24" si="0">F10*E10</f>
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ref="H10:H24" si="1">((E10-$F$28)^2)*F10</f>
+        <v>73.959094229364496</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ref="I10:I24" si="2">(EXP(-$F$32)*$F$32^E10)/FACT(E10)</f>
+        <v>3.3636066825848592E-3</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ref="J10:J24" si="3">$F$26*I10</f>
+        <v>0.49781378902255918</v>
+      </c>
+      <c r="K10">
+        <f>J12</f>
+        <v>4.9721577327296185</v>
+      </c>
+      <c r="L10">
+        <f>F12</f>
+        <v>7</v>
+      </c>
+      <c r="M10">
+        <f>((L10-K10)^2)/K10</f>
+        <v>0.82703415337364883</v>
+      </c>
+    </row>
+    <row r="11" spans="5:13">
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>103.26953981008033</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>1.3019365634329426E-2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>1.926866113880755</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="K11:K19" si="4">J13</f>
+        <v>9.6227570020491164</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ref="L11:L19" si="5">F13</f>
+        <v>13</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M10:M21" si="6">((L11-K11)^2)/K11</f>
+        <v>1.1852913115003809</v>
+      </c>
+    </row>
+    <row r="12" spans="5:13">
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>116.58655953250545</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>3.3595660356281205E-2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>4.9721577327296185</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="4"/>
+        <v>14.898554277303843</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="6"/>
+        <v>1.7467969023853873</v>
+      </c>
+    </row>
+    <row r="13" spans="5:13">
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>123.40978816654489</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>6.5018628392223762E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>9.6227570020491164</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="4"/>
+        <v>19.222394675671946</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="6"/>
+        <v>0.16438538186288629</v>
+      </c>
+    </row>
+    <row r="14" spans="5:13">
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>86.617969320671989</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0.10066590727908002</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>14.898554277303843</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="4"/>
+        <v>21.258081260188774</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="6"/>
+        <v>0.49934391387771976</v>
+      </c>
+    </row>
+    <row r="15" spans="5:13">
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>21</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>24.543462381300202</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>0.12988104510589152</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>19.222394675671946</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="4"/>
+        <v>20.570681914420117</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="6"/>
+        <v>2.098805523322131</v>
+      </c>
+    </row>
+    <row r="16" spans="5:13">
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>18</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>126</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0.11833455076698207</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>0.14363568419046469</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>21.258081260188774</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>17.69378688906578</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="6"/>
+        <v>0.16214245393359153</v>
+      </c>
+    </row>
+    <row r="17" spans="4:15">
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>112</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>11.821767713659616</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>0.13899109401635215</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>20.570681914420117</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="4"/>
+        <v>13.697313788639725</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="6"/>
+        <v>3.5499407207154048E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:15">
+      <c r="E18">
+        <v>9</v>
+      </c>
+      <c r="F18">
+        <v>16</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>58.915997078159265</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>0.11955261411530933</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>17.69378688906578</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="4"/>
+        <v>9.6395627048868526</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="6"/>
+        <v>4.2433507204099732E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="4:15">
+      <c r="E19">
+        <v>10</v>
+      </c>
+      <c r="F19">
+        <v>13</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>110.7611395178963</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>9.2549417490808958E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>13.697313788639725</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="4"/>
+        <v>6.2185724656686423</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="6"/>
+        <v>0.23878773822829302</v>
+      </c>
+    </row>
+    <row r="20" spans="4:15">
+      <c r="E20">
+        <v>11</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>99</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>138.22132943754568</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>6.5132180438424683E-2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>9.6395627048868526</v>
+      </c>
+      <c r="K20">
+        <f>SUM(J22:J24)</f>
+        <v>6.8074355467040357</v>
+      </c>
+      <c r="L20">
+        <f>SUM(F22:F24)</f>
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="6"/>
+        <v>0.47989044230775246</v>
+      </c>
+    </row>
+    <row r="21" spans="4:15">
+      <c r="E21">
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>120.97881665449235</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>4.2017381524788122E-2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>6.2185724656686423</v>
+      </c>
+    </row>
+    <row r="22" spans="4:15">
+      <c r="E22">
+        <v>13</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>105.10080350620893</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>2.5020745458033913E-2</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>3.7030703277890193</v>
+      </c>
+    </row>
+    <row r="23" spans="4:15">
+      <c r="E23">
+        <v>14</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>47.87143900657415</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>1.3835243972244345E-2</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>2.0476161078921629</v>
+      </c>
+    </row>
+    <row r="24" spans="4:15">
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>62.709276844411988</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>7.1401966961003637E-3</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>1.0567491110228537</v>
+      </c>
+    </row>
+    <row r="25" spans="4:15">
+      <c r="M25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="4:15">
+      <c r="D26" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9">
+        <f>SUM(F9:F24)</f>
+        <v>148</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" ref="G26:M26" si="7">SUM(G9:G24)</f>
+        <v>1048</v>
+      </c>
+      <c r="H26" s="9">
+        <f t="shared" si="7"/>
+        <v>1235.0270270270269</v>
+      </c>
+      <c r="I26" s="9">
+        <f t="shared" si="7"/>
+        <v>0.99385327216627861</v>
+      </c>
+      <c r="J26" s="9">
+        <f t="shared" si="7"/>
+        <v>147.09028428060927</v>
+      </c>
+      <c r="K26" s="9">
+        <f t="shared" si="7"/>
+        <v>147.09028428060924</v>
+      </c>
+      <c r="L26" s="9">
+        <f t="shared" si="7"/>
+        <v>148</v>
+      </c>
+      <c r="M26" s="9">
+        <f t="shared" si="7"/>
+        <v>15.656128440251953</v>
+      </c>
+    </row>
+    <row r="27" spans="4:15">
+      <c r="M27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="4:15">
+      <c r="E28" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="6">
+        <f>G26/F26</f>
+        <v>7.0810810810810807</v>
+      </c>
+    </row>
+    <row r="29" spans="4:15">
+      <c r="E29" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="6">
+        <f>H26/(F26-1)</f>
+        <v>8.4015444015444007</v>
+      </c>
+    </row>
+    <row r="30" spans="4:15">
+      <c r="E30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F30" s="6">
+        <f>SQRT(F29)</f>
+        <v>2.8985417715714226</v>
+      </c>
+    </row>
+    <row r="31" spans="4:15">
+      <c r="E31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="6">
+        <f>F30/F28</f>
+        <v>0.40933605171046811</v>
+      </c>
+    </row>
+    <row r="32" spans="4:15">
+      <c r="E32" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" s="10">
+        <f>(F28+F29)/2</f>
+        <v>7.7413127413127407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>